<commit_message>
before updating setup to split by sex
</commit_message>
<xml_diff>
--- a/raw_data/local_continuum/Jacksonville.xlsx
+++ b/raw_data/local_continuum/Jacksonville.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Dropbox/Documents_local/Hopkins/PhD/EHE/Suppression data/22. Jacksonville/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Fojo\CloudStation\Projects\Ending HIV\Ending_HIV\raw_data\local_continuum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A629E1-8A68-DE48-BA28-EBA39B98D3C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7760" yWindow="540" windowWidth="30480" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7764" yWindow="540" windowWidth="30480" windowHeight="19440" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Stratified_Data" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Comments" sheetId="2" r:id="rId4"/>
     <sheet name="Indicator definitions" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,17 +36,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={28E39B91-F9E6-014F-8597-340410927FF3}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{28E39B91-F9E6-014F-8597-340410927FF3}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     3 months</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -55,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>Total</t>
   </si>
@@ -223,17 +231,23 @@
   </si>
   <si>
     <t>Duval County</t>
+  </si>
+  <si>
+    <t>Florida epi profile tables</t>
+  </si>
+  <si>
+    <t>http://www.floridahealth.gov/diseases-and-conditions/aids/surveillance/epi-profiles/index.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,12 +277,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -863,22 +871,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -901,7 +909,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -924,7 +932,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -942,7 +950,7 @@
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
     </row>
-    <row r="4" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -960,7 +968,7 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
@@ -980,7 +988,7 @@
       <c r="P5" s="10"/>
       <c r="U5" s="10"/>
     </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -998,7 +1006,7 @@
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
     </row>
-    <row r="7" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1016,7 +1024,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1035,7 +1043,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1055,7 +1063,7 @@
       <c r="O9" s="15"/>
       <c r="P9" s="13"/>
     </row>
-    <row r="10" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1074,7 +1082,7 @@
       <c r="N10" s="22"/>
       <c r="O10" s="10"/>
     </row>
-    <row r="11" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1100,7 @@
       <c r="M11" s="21"/>
       <c r="N11" s="22"/>
     </row>
-    <row r="12" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
@@ -1111,7 +1119,7 @@
       <c r="N12" s="22"/>
       <c r="P12" s="14"/>
     </row>
-    <row r="13" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1129,7 +1137,7 @@
       <c r="M13" s="24"/>
       <c r="N13" s="22"/>
     </row>
-    <row r="14" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1147,7 +1155,7 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1174,7 @@
       <c r="N15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -1185,7 +1193,7 @@
       <c r="N16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1203,7 +1211,7 @@
       <c r="M17" s="23"/>
       <c r="N17" s="23"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1223,7 +1231,7 @@
       <c r="V18" s="31"/>
       <c r="W18" s="31"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H19" s="28"/>
       <c r="I19" s="29"/>
       <c r="J19" s="28"/>
@@ -1241,7 +1249,7 @@
       <c r="V19" s="31"/>
       <c r="W19" s="31"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>23</v>
       </c>
@@ -1267,7 +1275,7 @@
       <c r="Y20" s="31"/>
       <c r="Z20" s="31"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B21" s="79" t="s">
         <v>54</v>
       </c>
@@ -1295,7 +1303,7 @@
       <c r="Y21" s="31"/>
       <c r="Z21" s="31"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B22" s="64" t="s">
         <v>53</v>
       </c>
@@ -1324,7 +1332,7 @@
       <c r="Y22" s="31"/>
       <c r="Z22" s="31"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -1347,7 +1355,7 @@
       <c r="Y23" s="31"/>
       <c r="Z23" s="31"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -1370,7 +1378,7 @@
       <c r="Y24" s="31"/>
       <c r="Z24" s="31"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -1393,7 +1401,7 @@
       <c r="Y25" s="31"/>
       <c r="Z25" s="31"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -1416,7 +1424,7 @@
       <c r="Y26" s="31"/>
       <c r="Z26" s="31"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F27" s="31"/>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -1439,7 +1447,7 @@
       <c r="Y27" s="31"/>
       <c r="Z27" s="31"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
@@ -1462,7 +1470,7 @@
       <c r="Y28" s="31"/>
       <c r="Z28" s="31"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
@@ -1485,7 +1493,7 @@
       <c r="Y29" s="31"/>
       <c r="Z29" s="31"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F30" s="31" t="s">
         <v>23</v>
       </c>
@@ -1510,7 +1518,7 @@
       <c r="Y30" s="31"/>
       <c r="Z30" s="31"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
       <c r="H31" s="31"/>
@@ -1533,7 +1541,7 @@
       <c r="Y31" s="31"/>
       <c r="Z31" s="31"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
       <c r="H32" s="31"/>
@@ -1556,7 +1564,7 @@
       <c r="Y32" s="31"/>
       <c r="Z32" s="31"/>
     </row>
-    <row r="33" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -1577,7 +1585,7 @@
       <c r="W33" s="31"/>
       <c r="Z33" s="31"/>
     </row>
-    <row r="34" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F34" s="31"/>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -1588,7 +1596,7 @@
       <c r="Y34" s="31"/>
       <c r="Z34" s="31"/>
     </row>
-    <row r="35" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F35" s="31"/>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -1599,7 +1607,7 @@
       <c r="Y35" s="31"/>
       <c r="Z35" s="31"/>
     </row>
-    <row r="36" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F36" s="31"/>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -1622,7 +1630,7 @@
       <c r="Y36" s="31"/>
       <c r="Z36" s="31"/>
     </row>
-    <row r="37" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F37" s="31"/>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -1641,7 +1649,7 @@
       <c r="Y37" s="31"/>
       <c r="Z37" s="31"/>
     </row>
-    <row r="38" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F38" s="31"/>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
@@ -1660,7 +1668,7 @@
       <c r="Y38" s="31"/>
       <c r="Z38" s="31"/>
     </row>
-    <row r="39" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F39" s="31"/>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -1679,7 +1687,7 @@
       <c r="Y39" s="31"/>
       <c r="Z39" s="31"/>
     </row>
-    <row r="40" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F40" s="31"/>
       <c r="G40" s="31"/>
       <c r="H40" s="31"/>
@@ -1696,7 +1704,7 @@
       <c r="W40" s="31"/>
       <c r="X40" s="31"/>
     </row>
-    <row r="41" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F41" s="31"/>
       <c r="G41" s="31"/>
       <c r="H41" s="31"/>
@@ -1709,7 +1717,7 @@
       <c r="O41" s="31"/>
       <c r="X41" s="31"/>
     </row>
-    <row r="42" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F42" s="31"/>
       <c r="G42" s="31"/>
       <c r="H42" s="31"/>
@@ -1723,7 +1731,7 @@
       <c r="T42" s="31"/>
       <c r="X42" s="31"/>
     </row>
-    <row r="43" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F43" s="31"/>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
@@ -1732,7 +1740,7 @@
       <c r="K43" s="31"/>
       <c r="X43" s="31"/>
     </row>
-    <row r="44" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F44" s="31"/>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
@@ -1741,7 +1749,7 @@
       <c r="K44" s="31"/>
       <c r="X44" s="31"/>
     </row>
-    <row r="45" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F45" s="31"/>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
@@ -1753,7 +1761,7 @@
       <c r="W45" s="31"/>
       <c r="X45" s="31"/>
     </row>
-    <row r="46" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F46" s="31"/>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
@@ -1765,7 +1773,7 @@
       <c r="W46" s="31"/>
       <c r="X46" s="31"/>
     </row>
-    <row r="47" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F47" s="31"/>
       <c r="G47" s="31"/>
       <c r="H47" s="31"/>
@@ -1781,7 +1789,7 @@
       <c r="W47" s="31"/>
       <c r="X47" s="31"/>
     </row>
-    <row r="48" spans="6:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:26" x14ac:dyDescent="0.3">
       <c r="F48" s="31"/>
       <c r="G48" s="31"/>
       <c r="H48" s="31"/>
@@ -1802,7 +1810,7 @@
       <c r="W48" s="31"/>
       <c r="X48" s="31"/>
     </row>
-    <row r="49" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F49" s="31"/>
       <c r="G49" s="31"/>
       <c r="H49" s="31"/>
@@ -1823,7 +1831,7 @@
       <c r="W49" s="31"/>
       <c r="X49" s="31"/>
     </row>
-    <row r="50" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F50" s="31"/>
       <c r="G50" s="31"/>
       <c r="H50" s="31"/>
@@ -1844,7 +1852,7 @@
       <c r="W50" s="31"/>
       <c r="X50" s="31"/>
     </row>
-    <row r="51" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F51" s="31"/>
       <c r="G51" s="31"/>
       <c r="H51" s="31"/>
@@ -1865,7 +1873,7 @@
       <c r="W51" s="31"/>
       <c r="X51" s="31"/>
     </row>
-    <row r="52" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F52" s="31"/>
       <c r="G52" s="31"/>
       <c r="H52" s="31"/>
@@ -1886,7 +1894,7 @@
       <c r="W52" s="31"/>
       <c r="X52" s="31"/>
     </row>
-    <row r="53" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F53" s="31"/>
       <c r="G53" s="31"/>
       <c r="H53" s="31"/>
@@ -1907,7 +1915,7 @@
       <c r="W53" s="31"/>
       <c r="X53" s="31"/>
     </row>
-    <row r="54" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F54" s="31"/>
       <c r="G54" s="31"/>
       <c r="H54" s="31"/>
@@ -1928,7 +1936,7 @@
       <c r="W54" s="31"/>
       <c r="X54" s="31"/>
     </row>
-    <row r="55" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F55" s="31"/>
       <c r="G55" s="31"/>
       <c r="H55" s="31"/>
@@ -1949,7 +1957,7 @@
       <c r="W55" s="31"/>
       <c r="X55" s="31"/>
     </row>
-    <row r="56" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F56" s="31"/>
       <c r="G56" s="31"/>
       <c r="H56" s="31"/>
@@ -1970,7 +1978,7 @@
       <c r="W56" s="31"/>
       <c r="X56" s="31"/>
     </row>
-    <row r="57" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F57" s="31"/>
       <c r="G57" s="31"/>
       <c r="H57" s="31"/>
@@ -1991,7 +1999,7 @@
       <c r="W57" s="31"/>
       <c r="X57" s="31"/>
     </row>
-    <row r="58" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F58" s="31"/>
       <c r="G58" s="31"/>
       <c r="H58" s="31"/>
@@ -2012,7 +2020,7 @@
       <c r="W58" s="31"/>
       <c r="X58" s="31"/>
     </row>
-    <row r="59" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F59" s="31"/>
       <c r="G59" s="31"/>
       <c r="H59" s="31"/>
@@ -2033,7 +2041,7 @@
       <c r="W59" s="31"/>
       <c r="X59" s="31"/>
     </row>
-    <row r="60" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F60" s="31"/>
       <c r="G60" s="31"/>
       <c r="H60" s="31"/>
@@ -2054,7 +2062,7 @@
       <c r="W60" s="31"/>
       <c r="X60" s="31"/>
     </row>
-    <row r="61" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F61" s="31"/>
       <c r="G61" s="31"/>
       <c r="H61" s="31"/>
@@ -2075,7 +2083,7 @@
       <c r="W61" s="31"/>
       <c r="X61" s="31"/>
     </row>
-    <row r="62" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F62" s="31"/>
       <c r="G62" s="31"/>
       <c r="H62" s="31"/>
@@ -2096,7 +2104,7 @@
       <c r="W62" s="31"/>
       <c r="X62" s="31"/>
     </row>
-    <row r="63" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F63" s="31"/>
       <c r="G63" s="31"/>
       <c r="H63" s="31"/>
@@ -2117,7 +2125,7 @@
       <c r="W63" s="31"/>
       <c r="X63" s="31"/>
     </row>
-    <row r="64" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F64" s="31"/>
       <c r="G64" s="31"/>
       <c r="H64" s="31"/>
@@ -2138,7 +2146,7 @@
       <c r="W64" s="31"/>
       <c r="X64" s="31"/>
     </row>
-    <row r="65" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="65" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F65" s="31"/>
       <c r="G65" s="31"/>
       <c r="H65" s="31"/>
@@ -2159,7 +2167,7 @@
       <c r="W65" s="31"/>
       <c r="X65" s="31"/>
     </row>
-    <row r="66" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="66" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F66" s="31"/>
       <c r="G66" s="31"/>
       <c r="H66" s="31"/>
@@ -2180,7 +2188,7 @@
       <c r="W66" s="31"/>
       <c r="X66" s="31"/>
     </row>
-    <row r="67" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F67" s="31"/>
       <c r="G67" s="31"/>
       <c r="H67" s="31"/>
@@ -2201,7 +2209,7 @@
       <c r="W67" s="31"/>
       <c r="X67" s="31"/>
     </row>
-    <row r="68" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="68" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F68" s="31"/>
       <c r="G68" s="31"/>
       <c r="H68" s="31"/>
@@ -2222,7 +2230,7 @@
       <c r="W68" s="31"/>
       <c r="X68" s="31"/>
     </row>
-    <row r="69" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="69" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F69" s="31"/>
       <c r="G69" s="31"/>
       <c r="H69" s="31"/>
@@ -2243,7 +2251,7 @@
       <c r="W69" s="31"/>
       <c r="X69" s="31"/>
     </row>
-    <row r="70" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="70" spans="6:24" x14ac:dyDescent="0.3">
       <c r="F70" s="31"/>
       <c r="G70" s="31"/>
       <c r="H70" s="31"/>
@@ -2264,7 +2272,7 @@
       <c r="W70" s="31"/>
       <c r="X70" s="31"/>
     </row>
-    <row r="71" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="71" spans="6:24" x14ac:dyDescent="0.3">
       <c r="L71" s="31"/>
       <c r="M71" s="31"/>
       <c r="N71" s="31"/>
@@ -2278,7 +2286,7 @@
       <c r="V71" s="31"/>
       <c r="W71" s="31"/>
     </row>
-    <row r="72" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="72" spans="6:24" x14ac:dyDescent="0.3">
       <c r="L72" s="31"/>
       <c r="M72" s="31"/>
       <c r="N72" s="31"/>
@@ -2289,7 +2297,7 @@
       <c r="S72" s="31"/>
       <c r="T72" s="31"/>
     </row>
-    <row r="73" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="73" spans="6:24" x14ac:dyDescent="0.3">
       <c r="L73" s="31"/>
       <c r="M73" s="31"/>
       <c r="N73" s="31"/>
@@ -2300,7 +2308,7 @@
       <c r="S73" s="31"/>
       <c r="T73" s="31"/>
     </row>
-    <row r="74" spans="6:24" x14ac:dyDescent="0.2">
+    <row r="74" spans="6:24" x14ac:dyDescent="0.3">
       <c r="P74" s="31"/>
       <c r="Q74" s="31"/>
       <c r="R74" s="31"/>
@@ -2314,7 +2322,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC09810-A317-B740-AECD-B35CF86822F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -2324,15 +2332,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2373,7 +2381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2414,7 +2422,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -2455,7 +2463,7 @@
         <v>0.55100000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2496,7 +2504,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2537,7 +2545,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2578,7 +2586,7 @@
         <v>0.61499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -2619,7 +2627,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2660,7 +2668,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -2701,7 +2709,7 @@
         <v>0.42949999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2742,7 +2750,7 @@
         <v>0.44950000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2783,7 +2791,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2824,7 +2832,7 @@
         <v>0.58450000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -2865,7 +2873,7 @@
         <v>0.60549999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -2906,7 +2914,7 @@
         <v>0.58199999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2947,7 +2955,7 @@
         <v>0.504</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2988,7 +2996,7 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3029,7 +3037,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3037,55 +3045,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" s="64" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="64"/>
       <c r="D22" s="64"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37"/>
     </row>
   </sheetData>
@@ -3095,7 +3103,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -3108,12 +3116,12 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3136,7 +3144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2014</v>
       </c>
@@ -3163,7 +3171,7 @@
         <v>0.51421271159374005</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2015</v>
       </c>
@@ -3190,7 +3198,7 @@
         <v>0.55260678391959794</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2016</v>
       </c>
@@ -3217,7 +3225,7 @@
         <v>0.54784763084546295</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2017</v>
       </c>
@@ -3244,7 +3252,7 @@
         <v>0.54164749194661754</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2018</v>
       </c>
@@ -3271,7 +3279,7 @@
         <v>0.58720842738901424</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="79" t="s">
         <v>55</v>
       </c>
@@ -3285,49 +3293,51 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>48</v>
       </c>
@@ -3338,25 +3348,25 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="26"/>
       <c r="B11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="26"/>
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -3364,31 +3374,39 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{5E3C12A6-F884-4248-8E82-5FA74395CD99}"/>
+    <hyperlink ref="B13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9CD82F-C49B-E645-9ED1-742B79A009E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>28</v>
       </c>
@@ -3399,7 +3417,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>31</v>
       </c>
@@ -3408,7 +3426,7 @@
       </c>
       <c r="C2" s="43"/>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
         <v>30</v>
       </c>
@@ -3419,7 +3437,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>32</v>
       </c>
@@ -3428,7 +3446,7 @@
       </c>
       <c r="C4" s="43"/>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
         <v>33</v>
       </c>
@@ -3439,7 +3457,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="46" t="s">
         <v>39</v>
       </c>
@@ -3450,7 +3468,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>41</v>
       </c>
@@ -3461,69 +3479,69 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="36"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="36"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="36"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="36"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="36"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="36"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="36"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="36"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="36"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="36"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="36"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="36"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="36"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="36"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="36"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="36"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="36"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="36"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="36"/>
     </row>
   </sheetData>

</xml_diff>